<commit_message>
- CHG: Updated data templates.
</commit_message>
<xml_diff>
--- a/datatemplates/allele-calls.xlsx
+++ b/datatemplates/allele-calls.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\crop-trust\eggplant\data-templates\SP02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate3-bootstrap\datatemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- CHG: Updated data templates to include category tags to make automatic identification of template types easier. - ADD: Added more help content to the interface. - CHG: Changed automatic scrolling to group details section on the groups page. - CHG: Changed synonyms table to use JSON instead of multiple rows to store synonyms. This was caused by performance issues on all queries that included synonyms, because they had to use `GROUP_BY` and `GROUP_CONCAT` to join the synonyms into a single cell. - CHG: Restricted map during genotypic data export to only the markers included in the selected marker groups.
</commit_message>
<xml_diff>
--- a/datatemplates/allele-calls.xlsx
+++ b/datatemplates/allele-calls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate3-bootstrap\datatemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate\datatemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F220E40-EF8F-4B81-BA17-C096EB93E9C6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB6B508-4BE1-4934-AA03-B91068F30799}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="1" r:id="rId1"/>
@@ -947,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1210,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD428ACF-6755-4DFE-905C-713C69538445}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- ADD: Added the option to download the unbinned allele frequency data. - CHG: Unified 2 trait/compound chart and matrix chart into a single tab. Germinate will decide which one to show based on the number of selected traits/compounds. - ADD: Added further options for table page sizes: 250, 500. - CHG: Changed the way user registration works slightly. No new user account is approved straight away without the user verifying their email address. - CHG: Updated Bootstrap to v3.4.
</commit_message>
<xml_diff>
--- a/datatemplates/allele-calls.xlsx
+++ b/datatemplates/allele-calls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate\datatemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB6B508-4BE1-4934-AA03-B91068F30799}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7FAD23-D7DC-4560-A917-59CF01D7D266}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="1" r:id="rId1"/>
@@ -389,12 +389,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -442,13 +443,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="2" xr:uid="{37DE6626-7AEA-474F-A6DF-21A5375857BA}"/>
+    <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -595,8 +615,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -611,12 +631,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{899D81BA-0D15-4B0E-8198-E4AD18E04F51}" name="Table7" displayName="Table7" ref="A1:C16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{899D81BA-0D15-4B0E-8198-E4AD18E04F51}" name="Table7" displayName="Table7" ref="A1:C16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:C16" xr:uid="{C82FB4AE-F346-4BB9-8666-4FFBF429A944}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3F717630-B083-4BCD-9DDB-D3C1A46061E9}" name="LABEL" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{4459234A-B162-442C-A2B8-269CC581C79D}" name="DEFINITION" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{FD356382-869F-4EB0-A6F1-D92F30176135}" name="VALUE" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3F717630-B083-4BCD-9DDB-D3C1A46061E9}" name="LABEL" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4459234A-B162-442C-A2B8-269CC581C79D}" name="DEFINITION" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{FD356382-869F-4EB0-A6F1-D92F30176135}" name="VALUE" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -638,23 +658,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B17E13DC-A1BE-4337-94A3-20CE5E46A4FF}" name="Table8" displayName="Table8" ref="A1:G2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B17E13DC-A1BE-4337-94A3-20CE5E46A4FF}" name="Table8" displayName="Table8" ref="A1:G2" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G2" xr:uid="{2EA4EB1B-CF05-4161-8A4F-6C18B2873691}"/>
   <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{54E2AD32-A903-4B29-B50E-E1D57C66A08F}" name="Last Name" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2E4EEAB3-8C03-4513-BE97-157058BA75AA}" name="First Name" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{EB58BCE2-1172-40DD-9445-19879EBED028}" name="Email" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4E4F5E9A-70D3-45CA-977D-7BF61F7532EB}" name="Phone" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{EBFA69FE-7ABC-4DBF-BE40-87A581A669D7}" name="Contributor" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{551649BF-DFB9-4A79-9AB6-C84CF5A872B4}" name="Address" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{D291AC4F-D5AA-4E81-BCDB-9DC062C684E4}" name="Country" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{54E2AD32-A903-4B29-B50E-E1D57C66A08F}" name="Last Name" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{2E4EEAB3-8C03-4513-BE97-157058BA75AA}" name="First Name" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{EB58BCE2-1172-40DD-9445-19879EBED028}" name="Email" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{4E4F5E9A-70D3-45CA-977D-7BF61F7532EB}" name="Phone" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{EBFA69FE-7ABC-4DBF-BE40-87A581A669D7}" name="Contributor" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{551649BF-DFB9-4A79-9AB6-C84CF5A872B4}" name="Address" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{D291AC4F-D5AA-4E81-BCDB-9DC062C684E4}" name="Country" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C42421F5-3092-42FC-9D5E-D1D4D8B147C9}" name="Table5" displayName="Table5" ref="A3:A4" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C42421F5-3092-42FC-9D5E-D1D4D8B147C9}" name="Table5" displayName="Table5" ref="A3:A4" insertRow="1" totalsRowShown="0" headerRowCellStyle="Warning Text">
   <autoFilter ref="A3:A4" xr:uid="{388CDF32-3416-4F58-BD1E-AF0ACF62F192}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2A4EC3C5-80D3-40BA-BB1A-F78FFE0D4110}" name="Lines/Markers"/>
@@ -947,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +990,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -979,7 +999,7 @@
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1157,6 +1177,11 @@
       <c r="C24" s="6"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(C2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1283,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,11 +1328,16 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lines/Markers" prompt="Lines running across rows and markers running down columns." sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
   </dataValidations>

</xml_diff>